<commit_message>
Alu Sys Laptop Commit 30-06-2024
Alu Sys Laptop Commit 30-06-2024
</commit_message>
<xml_diff>
--- a/Budget/Cash Flow/Cash_Flow-2024.xlsx
+++ b/Budget/Cash Flow/Cash_Flow-2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A.Ouf\Odoo\Budget\Cash Flow\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\A.Ouf\Odoo\Odoo\Budget\Cash Flow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B988ACBD-D785-4304-A522-F6C8DB952E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA20034D-A5B2-46B9-8788-7B16B510C2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="931" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="931" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024" sheetId="16" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="95">
   <si>
     <t>2024</t>
   </si>
@@ -361,7 +361,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _ج_._م_._‏_-;\-* #,##0.00\ _ج_._م_._‏_-;_-* &quot;-&quot;??\ _ج_._م_._‏_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,6 +443,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -507,7 +554,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -587,6 +634,59 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -20403,8 +20503,8 @@
   </sheetPr>
   <dimension ref="A1:AA53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -24939,34 +25039,29 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8148C1EC-E58E-47EB-AAAF-88DF02B16C2F}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A2:C43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B4" sqref="B4:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.75" customWidth="1"/>
-    <col min="2" max="2" width="50.75" customWidth="1"/>
+    <col min="2" max="2" width="60" customWidth="1"/>
     <col min="3" max="3" width="15.875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="20" t="s">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C4"/>
     </row>
     <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -25197,7 +25292,7 @@
         <v>-2739191</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
@@ -25205,7 +25300,7 @@
         <v>-55562138.240000002</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>30</v>
       </c>
@@ -25213,7 +25308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
@@ -25221,7 +25316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
@@ -25229,7 +25324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>33</v>
       </c>
@@ -25237,7 +25332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
         <v>31</v>
       </c>
@@ -25245,7 +25340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
         <v>32</v>
       </c>
@@ -25253,7 +25348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>34</v>
       </c>
@@ -25261,7 +25356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
         <v>31</v>
       </c>
@@ -25269,7 +25364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
         <v>32</v>
       </c>
@@ -25277,7 +25372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="C39"/>
     </row>
     <row r="40" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -28412,8 +28507,8 @@
   </sheetPr>
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -28614,7 +28709,7 @@
         <v>402836242.80000001</v>
       </c>
       <c r="N5" s="26">
-        <f t="shared" ref="N4:N36" si="0">D5+F5+H5+J5+L5</f>
+        <f t="shared" ref="N5" si="0">D5+F5+H5+J5+L5</f>
         <v>93264007.049636424</v>
       </c>
       <c r="O5" s="26">
@@ -28665,7 +28760,7 @@
         <v>-16678683.65</v>
       </c>
       <c r="O6" s="26">
-        <f t="shared" ref="O6:O53" si="1">N6-M6</f>
+        <f t="shared" ref="O6:O52" si="1">N6-M6</f>
         <v>128512399.72999999</v>
       </c>
     </row>
@@ -28832,7 +28927,7 @@
         <v>-4097371.600000001</v>
       </c>
       <c r="N9" s="28">
-        <f t="shared" ref="N7:N53" si="2">D9+F9+H9+J9+L9</f>
+        <f t="shared" ref="N9:N53" si="2">D9+F9+H9+J9+L9</f>
         <v>-10826667.025750002</v>
       </c>
       <c r="O9" s="28">
@@ -30760,7 +30855,7 @@
       </c>
       <c r="D44" s="25">
         <f>SUM(D45:D46)</f>
-        <v>11485663.899999999</v>
+        <v>0</v>
       </c>
       <c r="E44" s="25">
         <f>IF(VLOOKUP($B44,'2'!$B$4:$C$337,2,FALSE)&lt;&gt;"",VLOOKUP($B44,'2'!$B$4:$C$337,2,FALSE),0)</f>
@@ -30800,11 +30895,11 @@
       </c>
       <c r="N44" s="25">
         <f>SUM(N45:N46)</f>
-        <v>-28126599.149999976</v>
+        <v>-39612263.049999952</v>
       </c>
       <c r="O44" s="25">
         <f>D44+F44+H44+J44+L44</f>
-        <v>-28126599.149999999</v>
+        <v>-39612263.049999997</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="27.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -30818,10 +30913,7 @@
         <f>IF(VLOOKUP($B45,'1'!$B$4:$C$336,2,FALSE)&lt;&gt;"",VLOOKUP($B45,'1'!$B$4:$C$336,2,FALSE),0)</f>
         <v>64195255.509999998</v>
       </c>
-      <c r="D45" s="26">
-        <f>IF(VLOOKUP($B45,'1'!$B$4:$C$336,2,FALSE)&lt;&gt;"",VLOOKUP($B45,'1'!$B$4:$C$336,2,FALSE),0)</f>
-        <v>64195255.509999998</v>
-      </c>
+      <c r="D45" s="26"/>
       <c r="E45" s="26">
         <f>IF(VLOOKUP($B45,'2'!$B$4:$C$337,2,FALSE)&lt;&gt;"",VLOOKUP($B45,'2'!$B$4:$C$337,2,FALSE),0)</f>
         <v>77940760.179999992</v>
@@ -30860,11 +30952,11 @@
       </c>
       <c r="N45" s="26">
         <f t="shared" si="2"/>
-        <v>539957208.98000002</v>
+        <v>475761953.47000003</v>
       </c>
       <c r="O45" s="26">
         <f t="shared" si="1"/>
-        <v>380868542.14999998</v>
+        <v>316673286.63999999</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30878,10 +30970,7 @@
         <f>IF(VLOOKUP($B46,'1'!$B$4:$C$336,2,FALSE)&lt;&gt;"",VLOOKUP($B46,'1'!$B$4:$C$336,2,FALSE),0)</f>
         <v>-52709591.609999999</v>
       </c>
-      <c r="D46" s="26">
-        <f>IF(VLOOKUP($B46,'1'!$B$4:$C$336,2,FALSE)&lt;&gt;"",VLOOKUP($B46,'1'!$B$4:$C$336,2,FALSE),0)</f>
-        <v>-52709591.609999999</v>
-      </c>
+      <c r="D46" s="26"/>
       <c r="E46" s="26">
         <f>IF(VLOOKUP($B46,'2'!$B$4:$C$337,2,FALSE)&lt;&gt;"",VLOOKUP($B46,'2'!$B$4:$C$337,2,FALSE),0)</f>
         <v>-79290371.609999999</v>
@@ -30920,11 +31009,11 @@
       </c>
       <c r="N46" s="26">
         <f t="shared" si="2"/>
-        <v>-568083808.13</v>
+        <v>-515374216.51999998</v>
       </c>
       <c r="O46" s="26">
         <f t="shared" si="1"/>
-        <v>-390018955.44999999</v>
+        <v>-337309363.83999997</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -31059,10 +31148,7 @@
         <f>C13+C39</f>
         <v>49180157.810000002</v>
       </c>
-      <c r="D50" s="12">
-        <f>D13+D39</f>
-        <v>21254302.874249998</v>
-      </c>
+      <c r="D50" s="12"/>
       <c r="E50" s="12">
         <v>28760602.36999999</v>
       </c>
@@ -31092,11 +31178,11 @@
       </c>
       <c r="N50" s="12">
         <f t="shared" si="2"/>
-        <v>131162811.89425001</v>
+        <v>109908509.02000001</v>
       </c>
       <c r="O50" s="12">
         <f t="shared" si="1"/>
-        <v>102386414.19424999</v>
+        <v>81132111.319999993</v>
       </c>
     </row>
     <row r="51" spans="2:15" ht="18" x14ac:dyDescent="0.2">
@@ -31107,10 +31193,7 @@
         <f>C22</f>
         <v>-42983510.909999996</v>
       </c>
-      <c r="D51" s="12">
-        <f>D22</f>
-        <v>-1619120.15</v>
-      </c>
+      <c r="D51" s="12"/>
       <c r="E51" s="12">
         <v>36306860.700000003</v>
       </c>
@@ -31140,11 +31223,11 @@
       </c>
       <c r="N51" s="12">
         <f t="shared" si="2"/>
-        <v>133462221.62</v>
+        <v>135081341.77000001</v>
       </c>
       <c r="O51" s="12">
         <f t="shared" si="1"/>
-        <v>100588452.31999999</v>
+        <v>102207572.47</v>
       </c>
     </row>
     <row r="52" spans="2:15" ht="18" x14ac:dyDescent="0.2">
@@ -31155,10 +31238,7 @@
         <f>SUM(C50:C51)</f>
         <v>6196646.900000006</v>
       </c>
-      <c r="D52" s="12">
-        <f>SUM(D50:D51)</f>
-        <v>19635182.72425</v>
-      </c>
+      <c r="D52" s="12"/>
       <c r="E52" s="12">
         <v>-7546258.3300000131</v>
       </c>
@@ -31188,11 +31268,11 @@
       </c>
       <c r="N52" s="12">
         <f t="shared" si="2"/>
-        <v>-5537650.02575</v>
+        <v>-25172832.75</v>
       </c>
       <c r="O52" s="12">
         <f t="shared" si="1"/>
-        <v>-1440278.425750006</v>
+        <v>-21075461.150000006</v>
       </c>
     </row>
     <row r="53" spans="2:15" ht="18" x14ac:dyDescent="0.25">
@@ -31205,7 +31285,7 @@
       </c>
       <c r="D53" s="34">
         <f>D49+D52</f>
-        <v>24924199.724249996</v>
+        <v>5289016.9999999981</v>
       </c>
       <c r="E53" s="34">
         <v>-1349611.4300000053</v>
@@ -31236,21 +31316,21 @@
       </c>
       <c r="N53" s="34">
         <f t="shared" si="2"/>
-        <v>-14688063.325750016</v>
+        <v>-34323246.050000012</v>
       </c>
       <c r="O53" s="34">
         <f>D53+F53+H53+J53+L53</f>
-        <v>-14688063.325750016</v>
+        <v>-34323246.050000012</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:J1"/>
     <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.59055118110236227" bottom="0.15748031496062992" header="0.31496062992125984" footer="0.11811023622047245"/>
@@ -31653,15 +31733,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50.75" customWidth="1"/>
-    <col min="3" max="3" width="16.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="102.5" customWidth="1"/>
+    <col min="3" max="3" width="22" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -31674,396 +31754,404 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="43">
         <v>5289016.9999999981</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="45">
         <v>21967700.649999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="45">
         <v>-16678683.65</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B8" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="47">
         <v>5289016.9999999981</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+    <row r="9" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+    </row>
+    <row r="10" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="43">
         <v>-29302777.950000111</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="51">
         <v>-39396775.950000107</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B12" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+      <c r="C12" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B13" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="45">
         <v>462448699.44</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="45">
         <v>46264640</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="45">
         <v>52862538.439999998</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="45">
         <v>363321521</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="2" t="s">
+    <row r="17" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B17" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="45">
         <v>462448699.44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+    <row r="18" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B18" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="45">
         <v>-20566.22000002861</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="45">
         <v>-20566.22000002861</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B20" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="45">
         <v>-20566.22000002861</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="2" t="s">
+    <row r="21" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B21" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="45">
         <v>-501824909.17000008</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="45">
         <v>-91186708</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="45">
         <v>-30620092.619999971</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="45">
         <v>-10904598.109999999</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="45">
         <v>-193252445.44000009</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="45">
         <v>-84340862</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="45">
         <v>-7785880</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="45">
         <v>-34570806</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="44" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="45">
         <v>-14789459</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="45">
         <v>-34123773</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="45">
         <v>-250285</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B32" s="2" t="s">
+    <row r="32" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B32" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="45">
         <v>-501824909.17000008</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B34" s="2" t="s">
+      <c r="C33" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B35" s="2" t="s">
+      <c r="C34" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="C35" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B37" s="2" t="s">
+      <c r="C36" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
+      <c r="C37" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B39" s="4" t="s">
+      <c r="C38" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B39" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="51">
         <v>10093998</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B40" s="2" t="s">
+    <row r="40" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="45">
         <v>10093998</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="45">
         <v>10093998</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B42" s="2" t="s">
+    <row r="42" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="45">
         <v>10093998</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B43" s="2" t="s">
+    <row r="43" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="C43" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="1" t="s">
+      <c r="C43" s="45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="48"/>
+      <c r="C44" s="49"/>
+    </row>
+    <row r="45" spans="1:3" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B45" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="43">
         <v>-24013760.949999992</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" ht="21" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="45">
         <v>349048740.02999997</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="45">
         <v>-373062500.98000002</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="3" t="s">
+    <row r="48" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B48" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="8">
+      <c r="C48" s="47">
         <v>-24013760.949999992</v>
       </c>
     </row>
@@ -32561,7 +32649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E178EDF-0F5D-4439-95A0-F8E7FAD41838}">
   <dimension ref="C3:O7"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
@@ -34921,411 +35009,592 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9077094E-0A70-4EAD-9452-81544966CB4B}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.75" customWidth="1"/>
-    <col min="2" max="2" width="50.75" customWidth="1"/>
-    <col min="3" max="3" width="15.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.75" style="13" customWidth="1"/>
+    <col min="2" max="2" width="123.75" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="35.625" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="13"/>
+    <col min="6" max="6" width="16.875" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="5" t="s">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="18"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="18"/>
+    </row>
+    <row r="4" spans="1:4" ht="36" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="53" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
+      <c r="C4" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="36" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="56">
         <v>5289016.9999999981</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="D5" s="56">
+        <f>IF(VLOOKUP($B5,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B5,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>5289016.9999999981</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="35.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="58">
         <v>21967700.649999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="D6" s="58">
+        <f>IF(VLOOKUP($B6,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B6,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>21967700.649999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="58">
         <v>-16678683.65</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="D7" s="58">
+        <f>IF(VLOOKUP($B7,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B7,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>-16678683.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="35.25" x14ac:dyDescent="0.2">
+      <c r="B8" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="60">
         <v>5289016.9999999981</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="D8" s="60">
+        <f>IF(VLOOKUP($B8,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B8,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>5289016.9999999981</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="B9" s="61"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+    </row>
+    <row r="10" spans="1:4" ht="36" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="56">
         <v>6196646.8999999994</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
+      <c r="D10" s="56">
+        <f>IF(VLOOKUP($B10,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B10,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>26659335.367249999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="36" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="64">
         <v>-3897351.100000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
+      <c r="D11" s="64">
+        <f>IF(VLOOKUP($B11,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B11,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>19635182.72425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="B12" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="2" t="s">
+      <c r="C12" s="58">
+        <v>0</v>
+      </c>
+      <c r="D12" s="58">
+        <f>IF(VLOOKUP($B12,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B12,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>3512076.3215000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="B13" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="58">
         <v>39086159.810000002</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="D13" s="58">
+        <f>IF(VLOOKUP($B13,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B13,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>21254302.874249998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="58">
         <v>590892</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="D14" s="58">
+        <f>IF(VLOOKUP($B14,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B14,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="58">
         <v>5021121.8900000006</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="D15" s="58">
+        <f>IF(VLOOKUP($B15,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B15,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>3720179.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="58">
         <v>10883958.92</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="D16" s="58">
+        <f>IF(VLOOKUP($B16,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B16,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>3512076.3215000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A17" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="58">
         <v>22590187</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="2" t="s">
+      <c r="D17" s="58">
+        <f>IF(VLOOKUP($B17,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B17,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>17534123.854249999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="B18" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="58">
         <v>39086159.810000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="2" t="s">
+      <c r="D18" s="58">
+        <f>IF(VLOOKUP($B18,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B18,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>21254302.874249998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="B19" s="57" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B20" s="2" t="s">
+      <c r="C19" s="58">
+        <v>0</v>
+      </c>
+      <c r="D19" s="58">
+        <f>IF(VLOOKUP($B19,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B19,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="B20" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="58">
         <v>-42983510.909999996</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="D20" s="58">
+        <f>IF(VLOOKUP($B20,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B20,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>-1619120.15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="58">
         <v>-9255999</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="D21" s="58">
+        <f>IF(VLOOKUP($B21,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B21,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="58">
         <v>-3434135.5200000019</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="D22" s="58">
+        <f>IF(VLOOKUP($B22,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B22,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>-1619120.15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="58">
         <v>-19119609.390000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="D23" s="58">
+        <f>IF(VLOOKUP($B23,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B23,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="58">
         <v>-4668939</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="D24" s="58">
+        <f>IF(VLOOKUP($B24,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B24,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="58">
         <v>-431011</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="D25" s="58">
+        <f>IF(VLOOKUP($B25,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B25,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="58">
         <v>-1913771</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="D26" s="58">
+        <f>IF(VLOOKUP($B26,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B26,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="58">
         <v>-2020737</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="D27" s="58">
+        <f>IF(VLOOKUP($B27,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B27,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="58">
         <v>-1889024</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="D28" s="58">
+        <f>IF(VLOOKUP($B28,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B28,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="58">
         <v>-250285</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="2" t="s">
+      <c r="D29" s="58">
+        <f>IF(VLOOKUP($B29,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B29,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="58">
         <v>-42983510.909999996</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="4" t="s">
+      <c r="D30" s="58">
+        <f>IF(VLOOKUP($B30,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B30,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="35.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="63" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15" x14ac:dyDescent="0.2">
-      <c r="B32" s="2" t="s">
+      <c r="C31" s="64">
+        <v>0</v>
+      </c>
+      <c r="D31" s="64">
+        <f>IF(VLOOKUP($B31,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B31,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B33" s="2" t="s">
+      <c r="C32" s="58">
+        <v>0</v>
+      </c>
+      <c r="D32" s="58">
+        <f>IF(VLOOKUP($B32,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B32,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
+      <c r="C33" s="58">
+        <v>0</v>
+      </c>
+      <c r="D33" s="58">
+        <f>IF(VLOOKUP($B33,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B33,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="35.25" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B35" s="2" t="s">
+      <c r="C34" s="64">
+        <v>0</v>
+      </c>
+      <c r="D34" s="64">
+        <f>IF(VLOOKUP($B34,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B34,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B36" s="2" t="s">
+      <c r="C35" s="58">
+        <v>0</v>
+      </c>
+      <c r="D35" s="58">
+        <f>IF(VLOOKUP($B35,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B35,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="C36" s="58">
+        <v>0</v>
+      </c>
+      <c r="D36" s="58">
+        <f>IF(VLOOKUP($B36,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B36,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="35.25" x14ac:dyDescent="0.2">
+      <c r="B37" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="64">
         <v>10093998</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B38" s="2" t="s">
+      <c r="D37" s="64">
+        <f>IF(VLOOKUP($B37,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B37,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="58">
         <v>10093998</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="D38" s="58">
+        <f>IF(VLOOKUP($B38,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B38,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="58">
         <v>10093998</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B40" s="2" t="s">
+      <c r="D39" s="58">
+        <f>IF(VLOOKUP($B39,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B39,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="58">
         <v>10093998</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B41" s="2" t="s">
+      <c r="D40" s="58">
+        <f>IF(VLOOKUP($B40,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B40,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="C41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="1" t="s">
+      <c r="C41" s="58">
+        <v>0</v>
+      </c>
+      <c r="D41" s="58">
+        <f>IF(VLOOKUP($B41,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B41,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="34.5" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62" t="e">
+        <f>IF(VLOOKUP($B42,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B42,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="36" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="56">
         <v>11485663.9</v>
       </c>
-      <c r="E43">
+      <c r="D43" s="56">
+        <f>IF(VLOOKUP($B43,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B43,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="E43" s="13">
         <v>65686942</v>
       </c>
-      <c r="F43" s="35">
+      <c r="F43" s="52">
         <f>E43-C44</f>
         <v>1491686.4900000021</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+    <row r="44" spans="1:6" ht="35.25" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="57" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="58">
         <v>64195255.509999998</v>
       </c>
-      <c r="F44" s="35">
+      <c r="D44" s="58">
+        <f>IF(VLOOKUP($B44,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B44,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+      <c r="F44" s="52">
         <f>E43-C14</f>
         <v>65096050</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+    <row r="45" spans="1:6" ht="34.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="57" t="s">
         <v>79</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="58">
         <v>-52709591.609999999</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B46" s="3" t="s">
+      <c r="D45" s="58">
+        <f>IF(VLOOKUP($B45,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE)&lt;&gt;"",VLOOKUP($B45,'2024 1,5-2024'!$B$4:$Z$336,3,FALSE),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="35.25" x14ac:dyDescent="0.2">
+      <c r="B46" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="8">
+      <c r="C46" s="60">
         <v>11485663.9</v>
+      </c>
+      <c r="D46" s="60">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>